<commit_message>
Build 2 - further development #16 documented Z80 instructions now 100% complete
</commit_message>
<xml_diff>
--- a/docs/instruction_coverage.xlsx
+++ b/docs/instruction_coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\box80\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F069CD55-C2D1-4E41-9B0C-A94F171FDBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE65378-2CF1-4F6B-90D5-3230B2D701B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="768" windowWidth="20076" windowHeight="11472" xr2:uid="{35671749-8C23-487D-B449-F5BA0CCE0876}"/>
   </bookViews>
@@ -36,42 +36,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Duncan Munro</author>
-  </authors>
-  <commentList>
-    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{BA27F63F-3D29-44FE-AB97-956E323FCE7F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Duncan Munro:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Includes 4 undocumented instructions</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>BOX80 - Instruction Coverage</t>
   </si>
@@ -79,9 +45,6 @@
     <t>Date/Time</t>
   </si>
   <si>
-    <t>Standard</t>
-  </si>
-  <si>
     <t>DD CB</t>
   </si>
   <si>
@@ -121,12 +84,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>%ALL</t>
-  </si>
-  <si>
-    <t>%STD</t>
-  </si>
-  <si>
     <t>Opcode</t>
   </si>
   <si>
@@ -197,6 +154,30 @@
   </si>
   <si>
     <t>IFF1/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = Undocumented</t>
+  </si>
+  <si>
+    <t>Documented</t>
+  </si>
+  <si>
+    <t>Undocumented</t>
+  </si>
+  <si>
+    <t>%undoc</t>
+  </si>
+  <si>
+    <t>Doc</t>
+  </si>
+  <si>
+    <t>Undoc</t>
+  </si>
+  <si>
+    <t>%doc</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
 </sst>
 </file>
@@ -206,7 +187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,33 +218,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -272,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -282,6 +286,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -289,6 +299,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -611,375 +626,769 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DE8576-3351-47DD-BEEA-F23B5608B549}">
-  <dimension ref="A1:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DE8576-3351-47DD-BEEA-F23B5608B549}">
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="20" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="8"/>
+      <c r="C3" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="9">
         <v>256</v>
       </c>
-      <c r="C3">
+      <c r="C5" s="9">
+        <v>248</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
+        <v>40</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9">
+        <v>31</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9">
+        <v>56</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
+        <v>40</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9">
+        <v>31</v>
+      </c>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9">
+        <f>SUM(B5:M5)</f>
+        <v>702</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
+        <v>8</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9">
+        <v>126</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
+        <v>225</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9">
+        <v>4</v>
+      </c>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9">
+        <v>126</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9">
+        <v>225</v>
+      </c>
+      <c r="O6" s="9">
+        <f>SUM(B6:M6)</f>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="10">
+        <f>SUM(O5:O6)</f>
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45107.833333333336</v>
+      </c>
+      <c r="B11">
+        <v>211</v>
+      </c>
+      <c r="C11">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>SUM(B11:N11)</f>
+        <v>279</v>
+      </c>
+      <c r="P11">
+        <f>SUM(B11,C11,E11,G11,I11,K11,M11)</f>
+        <v>279</v>
+      </c>
+      <c r="Q11">
+        <f>SUM(D11,F11,H11,J11,L11,N11)</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="4">
+        <f>O11/$O$7</f>
+        <v>0.23425692695214106</v>
+      </c>
+      <c r="S11" s="4">
+        <f>P11/$O$5</f>
+        <v>0.39743589743589741</v>
+      </c>
+      <c r="T11" s="4">
+        <f>Q11/$O$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45107.940972222219</v>
+      </c>
+      <c r="B12">
+        <v>247</v>
+      </c>
+      <c r="C12">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12:O18" si="0">SUM(B12:N12)</f>
+        <v>319</v>
+      </c>
+      <c r="P12">
+        <f t="shared" ref="P12:P17" si="1">SUM(B12,C12,E12,G12,I12,K12,M12)</f>
+        <v>319</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ref="Q12:Q17" si="2">SUM(D12,F12,H12,J12,L12,N12)</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <f t="shared" ref="R12:R17" si="3">O12/$O$7</f>
+        <v>0.26784214945424012</v>
+      </c>
+      <c r="S12" s="4">
+        <f t="shared" ref="S12:S17" si="4">P12/$O$5</f>
+        <v>0.45441595441595439</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" ref="T12:T17" si="5">Q12/$O$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45108.504166666666</v>
+      </c>
+      <c r="B13">
         <v>256</v>
       </c>
-      <c r="D3">
-        <v>40</v>
-      </c>
-      <c r="E3">
-        <v>21</v>
-      </c>
-      <c r="F3">
-        <v>56</v>
-      </c>
-      <c r="G3">
-        <v>40</v>
-      </c>
-      <c r="H3">
-        <v>21</v>
-      </c>
-      <c r="I3">
-        <f>SUM(B3:H3)</f>
-        <v>690</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C13">
+        <v>64</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
         <v>7</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>45107.833333333336</v>
-      </c>
-      <c r="B7">
-        <v>211</v>
-      </c>
-      <c r="C7">
-        <v>64</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <f t="shared" ref="I7:I12" si="0">SUM(B7:H7)</f>
-        <v>279</v>
-      </c>
-      <c r="J7" s="4">
-        <f t="shared" ref="J7:J12" si="1">B7/$B$3</f>
-        <v>0.82421875</v>
-      </c>
-      <c r="K7" s="4">
-        <f t="shared" ref="K7:K12" si="2">I7/$I$3</f>
-        <v>0.40434782608695652</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>45107.940972222219</v>
-      </c>
-      <c r="B8">
-        <v>247</v>
-      </c>
-      <c r="C8">
-        <v>64</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>319</v>
-      </c>
-      <c r="J8" s="4">
-        <f t="shared" si="1"/>
-        <v>0.96484375</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" si="2"/>
-        <v>0.46231884057971012</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>45108.504166666666</v>
-      </c>
-      <c r="B9">
-        <v>256</v>
-      </c>
-      <c r="C9">
-        <v>64</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
         <f t="shared" si="0"/>
         <v>328</v>
       </c>
-      <c r="J9" s="4">
+      <c r="P13">
         <f t="shared" si="1"/>
+        <v>328</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.27539882451721243</v>
+      </c>
+      <c r="S13" s="4">
+        <f t="shared" si="4"/>
+        <v>0.46723646723646722</v>
+      </c>
+      <c r="T13" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45108.909722222219</v>
+      </c>
+      <c r="B14">
+        <v>256</v>
+      </c>
+      <c r="C14">
+        <v>128</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>1</v>
       </c>
-      <c r="K9" s="4">
-        <f t="shared" si="2"/>
-        <v>0.47536231884057972</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>45108.909722222219</v>
-      </c>
-      <c r="B10">
-        <v>256</v>
-      </c>
-      <c r="C10">
-        <v>128</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
         <v>7</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
         <f t="shared" si="0"/>
         <v>392</v>
       </c>
-      <c r="J10" s="4">
+      <c r="P14">
         <f t="shared" si="1"/>
+        <v>392</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="4">
+        <f t="shared" si="3"/>
+        <v>0.32913518052057095</v>
+      </c>
+      <c r="S14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.55840455840455838</v>
+      </c>
+      <c r="T14" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45108.920138888891</v>
+      </c>
+      <c r="B15">
+        <v>256</v>
+      </c>
+      <c r="C15">
+        <v>248</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
         <v>1</v>
       </c>
-      <c r="K10" s="4">
-        <f t="shared" si="2"/>
-        <v>0.56811594202898552</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>45108.920138888891</v>
-      </c>
-      <c r="B11">
-        <v>256</v>
-      </c>
-      <c r="C11">
-        <v>256</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
         <v>7</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
         <f t="shared" si="0"/>
         <v>520</v>
       </c>
-      <c r="J11" s="4">
+      <c r="P15">
         <f t="shared" si="1"/>
+        <v>512</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="R15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.43660789252728799</v>
+      </c>
+      <c r="S15" s="4">
+        <f t="shared" si="4"/>
+        <v>0.72934472934472938</v>
+      </c>
+      <c r="T15" s="4">
+        <f t="shared" si="5"/>
+        <v>1.6359918200408999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45109.45</v>
+      </c>
+      <c r="B16">
+        <v>256</v>
+      </c>
+      <c r="C16">
+        <v>248</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
         <v>1</v>
       </c>
-      <c r="K11" s="4">
-        <f t="shared" si="2"/>
-        <v>0.75362318840579712</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>45109.45</v>
-      </c>
-      <c r="B12">
-        <v>256</v>
-      </c>
-      <c r="C12">
-        <v>256</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
         <v>23</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
         <f t="shared" si="0"/>
         <v>536</v>
       </c>
-      <c r="J12" s="4">
+      <c r="P16">
         <f t="shared" si="1"/>
+        <v>528</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="R16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.45004198152812763</v>
+      </c>
+      <c r="S16" s="4">
+        <f t="shared" si="4"/>
+        <v>0.75213675213675213</v>
+      </c>
+      <c r="T16" s="4">
+        <f t="shared" si="5"/>
+        <v>1.6359918200408999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>45109.614583333336</v>
+      </c>
+      <c r="B17">
+        <v>256</v>
+      </c>
+      <c r="C17">
+        <v>248</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
         <v>1</v>
       </c>
-      <c r="K12" s="4">
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>56</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>573</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="1"/>
+        <v>561</v>
+      </c>
+      <c r="Q17">
         <f t="shared" si="2"/>
-        <v>0.77681159420289858</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>45109.614583333336</v>
-      </c>
-      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="R17" s="4">
+        <f t="shared" si="3"/>
+        <v>0.48110831234256929</v>
+      </c>
+      <c r="S17" s="4">
+        <f t="shared" si="4"/>
+        <v>0.79914529914529919</v>
+      </c>
+      <c r="T17" s="4">
+        <f t="shared" si="5"/>
+        <v>2.4539877300613498E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45110.753472222219</v>
+      </c>
+      <c r="B18">
         <v>256</v>
       </c>
-      <c r="C13">
-        <v>256</v>
-      </c>
-      <c r="D13">
+      <c r="C18">
+        <v>248</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>40</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>31</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>56</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>40</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>31</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>714</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18" si="6">SUM(B18,C18,E18,G18,I18,K18,M18)</f>
+        <v>702</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" ref="Q18" si="7">SUM(D18,F18,H18,J18,L18,N18)</f>
+        <v>12</v>
+      </c>
+      <c r="R18" s="4">
+        <f t="shared" ref="R18" si="8">O18/$O$7</f>
+        <v>0.59949622166246852</v>
+      </c>
+      <c r="S18" s="4">
+        <f t="shared" ref="S18" si="9">P18/$O$5</f>
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>60</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ref="I13" si="3">SUM(B13:H13)</f>
-        <v>573</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" ref="J13" si="4">B13/$B$3</f>
-        <v>1</v>
-      </c>
-      <c r="K13" s="4">
-        <f t="shared" ref="K13" si="5">I13/$I$3</f>
-        <v>0.83043478260869563</v>
+      <c r="T18" s="4">
+        <f t="shared" ref="T18" si="10">Q18/$O$6</f>
+        <v>2.4539877300613498E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1000,111 +1409,111 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to opcode spreadsheet
</commit_message>
<xml_diff>
--- a/docs/instruction_coverage.xlsx
+++ b/docs/instruction_coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\box80\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE65378-2CF1-4F6B-90D5-3230B2D701B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60A8977-67C0-4068-8972-5E99B9FF05E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="768" windowWidth="20076" windowHeight="11472" xr2:uid="{35671749-8C23-487D-B449-F5BA0CCE0876}"/>
   </bookViews>
@@ -630,7 +630,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Buffering and terminal writes overhauled Much quicker, not missing any input characters but missing some screen output characters or doubling them up (all are OK in the log file)
</commit_message>
<xml_diff>
--- a/docs/instruction_coverage.xlsx
+++ b/docs/instruction_coverage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\box80\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60A8977-67C0-4068-8972-5E99B9FF05E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C5361E-D1FE-4E75-A278-110F875B2F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="768" windowWidth="20076" windowHeight="11472" xr2:uid="{35671749-8C23-487D-B449-F5BA0CCE0876}"/>
+    <workbookView xWindow="10080" yWindow="1710" windowWidth="16905" windowHeight="12990" activeTab="1" xr2:uid="{35671749-8C23-487D-B449-F5BA0CCE0876}"/>
   </bookViews>
   <sheets>
     <sheet name="Coverage" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>BOX80 - Instruction Coverage</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Interrupt enable flip flops not implemented, although IFF1 is shown as int_enabled</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>R register is not incremented unless the app is compiled with UPDATE_R_REG defined (10% performance penalty)</t>
   </si>
   <si>
@@ -178,6 +175,12 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>NMI</t>
+  </si>
+  <si>
+    <t>NMI is not enabled</t>
   </si>
 </sst>
 </file>
@@ -316,10 +319,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16C3FF11-951F-4ADF-ABC1-4F9C088C8F87}" name="Table1" displayName="Table1" ref="A4:C12" totalsRowShown="0">
-  <autoFilter ref="A4:C12" xr:uid="{16C3FF11-951F-4ADF-ABC1-4F9C088C8F87}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:C12">
-    <sortCondition ref="A4:A12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16C3FF11-951F-4ADF-ABC1-4F9C088C8F87}" name="Table1" displayName="Table1" ref="A4:C13" totalsRowShown="0">
+  <autoFilter ref="A4:C13" xr:uid="{16C3FF11-951F-4ADF-ABC1-4F9C088C8F87}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:C13">
+    <sortCondition ref="A4:A13"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{47B37D3D-E3F7-4B85-87CB-EBDF71A5DE16}" name="Opcode"/>
@@ -629,30 +632,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DE8576-3351-47DD-BEEA-F23B5608B549}">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="20" width="6.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="20" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
       <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="B5" s="9">
         <v>256</v>
@@ -686,9 +689,9 @@
         <v>702</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -720,7 +723,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
@@ -742,7 +745,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
         <v>3</v>
@@ -781,12 +784,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -828,22 +831,22 @@
         <v>14</v>
       </c>
       <c r="P10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45107.833333333336</v>
       </c>
@@ -911,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45107.940972222219</v>
       </c>
@@ -979,7 +982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45108.504166666666</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45108.909722222219</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45108.920138888891</v>
       </c>
@@ -1183,7 +1186,7 @@
         <v>1.6359918200408999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45109.45</v>
       </c>
@@ -1251,7 +1254,7 @@
         <v>1.6359918200408999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45109.614583333336</v>
       </c>
@@ -1319,7 +1322,7 @@
         <v>2.4539877300613498E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45110.753472222219</v>
       </c>
@@ -1394,30 +1397,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{347C0B75-B920-46EC-991B-2EA949989004}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="94.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1428,91 +1431,102 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>